<commit_message>
ATX view added to tables
</commit_message>
<xml_diff>
--- a/storage/app/excel/export-templates/ivp.xlsx
+++ b/storage/app/excel/export-templates/ivp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\home\erp-evolet\storage\app\excel\export-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43B5C94-0DF2-495E-A978-27639D3367DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CDF438-73A9-4CF6-87E6-2E381FAC1537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>БДМ</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Бренд</t>
+  </si>
+  <si>
+    <t>ATX</t>
+  </si>
+  <si>
+    <t>Наш АТХ</t>
   </si>
 </sst>
 </file>
@@ -529,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB10"/>
+  <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,25 +554,25 @@
     <col min="9" max="9" width="9.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="18.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="11.85546875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="13.42578125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="14.42578125" customWidth="1"/>
-    <col min="24" max="24" width="10.28515625" customWidth="1"/>
-    <col min="25" max="25" width="11.28515625" customWidth="1"/>
-    <col min="26" max="26" width="13.7109375" customWidth="1"/>
-    <col min="27" max="27" width="15.7109375" customWidth="1"/>
-    <col min="28" max="28" width="16.85546875" customWidth="1"/>
+    <col min="12" max="14" width="9.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" style="1" customWidth="1"/>
+    <col min="16" max="17" width="9.85546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" customWidth="1"/>
+    <col min="26" max="26" width="10.28515625" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" customWidth="1"/>
+    <col min="28" max="28" width="13.7109375" customWidth="1"/>
+    <col min="29" max="29" width="15.7109375" customWidth="1"/>
+    <col min="30" max="30" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -607,77 +613,83 @@
         <v>25</v>
       </c>
       <c r="N1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="T2"/>
-      <c r="U2"/>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="T3"/>
-      <c r="U3"/>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="T4"/>
-      <c r="U4"/>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="U8"/>
-      <c r="V8"/>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="W8"/>
+      <c r="X8"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="U9"/>
-      <c r="V9"/>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="W9"/>
+      <c r="X9"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="U10"/>
-      <c r="V10"/>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="W10"/>
+      <c r="X10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>